<commit_message>
latch implemented in software
</commit_message>
<xml_diff>
--- a/Hardware/RPI5-Scan2Go-HAT/Technische specificaties HAT.xlsx
+++ b/Hardware/RPI5-Scan2Go-HAT/Technische specificaties HAT.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/cr_tak_student_han_nl/Documents/S8 (afstuderen)/Software+Hardware/Hardware/RPI5-Scan2Go-HAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crtak\OneDrive - HAN\S8 (afstuderen)\Software+Hardware\Hardware\RPI5-Scan2Go-HAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="456" documentId="8_{471679F7-0749-465C-94AA-78C37701B0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39D9CF6D-B267-4744-9CE9-78D24EF40647}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9F6F5D-5FE1-436D-AB03-9F14B596A5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3420" yWindow="3420" windowWidth="17280" windowHeight="9960" xr2:uid="{A1EA83D2-A6D0-4FF4-A387-952356D5B8E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1EA83D2-A6D0-4FF4-A387-952356D5B8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="0">Blad1!$A$14</definedName>
+    <definedName name="_ftn1" localSheetId="0">Blad1!$A$13</definedName>
     <definedName name="_ftnref1" localSheetId="0">Blad1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>MoSCoW</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">De RPI afmetingen worden geïnspireerd op de volgende specificatie/richtlijnen: https://github.com/raspberrypi/hats </t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">De Raspberry Pi 5 word vanuit de printplaat gevoed via de GPIO pinnen. </t>
-  </si>
-  <si>
-    <t>T4.3</t>
   </si>
   <si>
     <t>Er worden soldeer jumpers geïnstalleerd op plekken waar functionaliteit kan worden geschakeld tussen RPI5 en RPI3 en RPI4, Hierbij is de standaard uitgaande van de RPI5.</t>
@@ -481,15 +475,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -566,13 +557,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>142987</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>11205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1590787</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>179093</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -627,13 +618,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4417807</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>11591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5736067</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>125505</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -688,13 +679,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1628887</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>3585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4343120</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>34065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -746,10 +737,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1069,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7C3E10-E9C9-4DAC-83DF-6861CB9F2522}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="A1:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,86 +1072,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="C4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1172,13 +1159,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1188,39 +1175,39 @@
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>33</v>
+      <c r="C8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1228,109 +1215,97 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="8" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="B17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>52</v>
+      <c r="D17" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>